<commit_message>
Progress on Sample 5
</commit_message>
<xml_diff>
--- a/TreeProcessing/measured_data/Book1.xlsx
+++ b/TreeProcessing/measured_data/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/Classes/CS898/FinalProject/trees/TreeProcessing/measured_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C3F35EC-CCC9-1241-9577-C9CDB746A264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA944796-AE40-CD43-992C-9463E9AE0D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{F265224F-3ACE-B541-9282-E588C9BB9A4C}"/>
+    <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{09C38D39-7E2D-FF43-8C19-60EBBA6C5EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,67 +378,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8621E653-F816-B544-BBEB-72463AA7D8C8}">
-  <dimension ref="A2:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA3B22A-9544-1A47-8359-584FF8E69E97}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>140</v>
+      </c>
+      <c r="B1">
+        <f>A1/3.141596</f>
+        <v>44.563336597067227</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="B2">
-        <f>A2/3.14</f>
-        <v>44.585987261146492</v>
+        <f t="shared" ref="B2:B6" si="0">A2/3.141596</f>
+        <v>21.326739657167888</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>67</v>
+        <v>50.5</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B7" si="0">A3/3.14</f>
-        <v>21.337579617834393</v>
+        <f t="shared" si="0"/>
+        <v>16.074632129656393</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>50.5</v>
+        <v>12.5</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>16.082802547770701</v>
+        <v>3.9788693390238596</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>12.5</v>
+        <v>146.30000000000001</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>3.9808917197452227</v>
+        <v>46.568686743935253</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>146.30000000000001</v>
+        <v>92.8</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>46.592356687898089</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>92.8</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>29.554140127388532</v>
+        <v>29.53912597291313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now have depth estimation for occluded trees
</commit_message>
<xml_diff>
--- a/TreeProcessing/measured_data/Book1.xlsx
+++ b/TreeProcessing/measured_data/Book1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/Classes/CS898/FinalProject/trees/TreeProcessing/measured_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA944796-AE40-CD43-992C-9463E9AE0D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A94B0-2689-4745-BB2B-CC14D953A363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{09C38D39-7E2D-FF43-8C19-60EBBA6C5EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,15 +32,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t>computed</t>
+  </si>
+  <si>
+    <t>percent err</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,66 +400,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA3B22A-9544-1A47-8359-584FF8E69E97}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>140</v>
       </c>
-      <c r="B1">
-        <f>A1/3.141596</f>
+      <c r="B2">
+        <f>A2/3.141596</f>
         <v>44.563336597067227</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>(C2 - B2)/B2</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>67</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B6" si="0">A2/3.141596</f>
+      <c r="B3">
+        <f t="shared" ref="B3:B7" si="0">A3/3.141596</f>
         <v>21.326739657167888</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C3" s="1">
+        <v>19.119</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="1">(C3 - B3)/B3</f>
+        <v>-0.10351979217910461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>50.5</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>16.074632129656393</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C4" s="1">
+        <v>15.936</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>-8.6242800792080618E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>12.5</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>3.9788693390238596</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="C5" s="1">
+        <v>3.87</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>-2.7361878400000077E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>146.30000000000001</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>46.568686743935253</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="C6" s="1">
+        <v>43.494</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>-6.602476812030085E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>92.8</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>29.53912597291313</v>
+      </c>
+      <c r="C7" s="1">
+        <v>149.08000000000001</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>4.0468656431034491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DBH estimate using segmentation
</commit_message>
<xml_diff>
--- a/TreeProcessing/measured_data/Book1.xlsx
+++ b/TreeProcessing/measured_data/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Documents/Classes/CS898/FinalProject/trees/TreeProcessing/measured_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03A94B0-2689-4745-BB2B-CC14D953A363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6A206F-443B-3945-9905-6180B6B04B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{09C38D39-7E2D-FF43-8C19-60EBBA6C5EFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15620" windowHeight="22400" xr2:uid="{09C38D39-7E2D-FF43-8C19-60EBBA6C5EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>measured</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>percent err</t>
+  </si>
+  <si>
+    <t>w/ the whole process for each sample</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA3B22A-9544-1A47-8359-584FF8E69E97}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,8 +434,8 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>(C2 - B2)/B2</f>
-        <v>-1</v>
+        <f>100*(C2 - B2)/B2</f>
+        <v>-100</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -447,8 +450,8 @@
         <v>19.119</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="1">(C3 - B3)/B3</f>
-        <v>-0.10351979217910461</v>
+        <f>100*(C3 - B3)/B3</f>
+        <v>-10.351979217910461</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -463,8 +466,8 @@
         <v>15.936</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>-8.6242800792080618E-3</v>
+        <f t="shared" ref="D4:D7" si="1">100*(C4 - B4)/B4</f>
+        <v>-0.86242800792080609</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -472,7 +475,7 @@
         <v>12.5</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>A5/3.141596</f>
         <v>3.9788693390238596</v>
       </c>
       <c r="C5" s="1">
@@ -480,7 +483,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-2.7361878400000077E-2</v>
+        <v>-2.7361878400000079</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -496,7 +499,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>-6.602476812030085E-2</v>
+        <v>-6.6024768120300834</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -508,11 +511,123 @@
         <v>29.53912597291313</v>
       </c>
       <c r="C7" s="1">
-        <v>149.08000000000001</v>
+        <v>28.29</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>4.0468656431034491</v>
+        <v>-4.2287167672413792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>140</v>
+      </c>
+      <c r="B13">
+        <f>A13/3.141596</f>
+        <v>44.563336597067227</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>100*(C13 - B13)/B13</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B18" si="2">A14/3.141596</f>
+        <v>21.326739657167888</v>
+      </c>
+      <c r="C14" s="1">
+        <v>19.119</v>
+      </c>
+      <c r="D14">
+        <f>100*(C14 - B14)/B14</f>
+        <v>-10.351979217910461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50.5</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>16.074632129656393</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15.936</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D18" si="3">100*(C15 - B15)/B15</f>
+        <v>-0.86242800792080609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12.5</v>
+      </c>
+      <c r="B16">
+        <f>A16/3.141596</f>
+        <v>3.9788693390238596</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.87</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>-2.7361878400000079</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:B18" si="4">A17/3.141596</f>
+        <v>46.568686743935253</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43.494</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>-6.6024768120300834</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>92.8</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>29.53912597291313</v>
+      </c>
+      <c r="C18" s="1">
+        <v>28.29</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>-4.2287167672413792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>